<commit_message>
Added some sample sketches
</commit_message>
<xml_diff>
--- a/Docu/registers.xlsx
+++ b/Docu/registers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Reg ID</t>
   </si>
@@ -162,15 +162,9 @@
     <t>//Custom Registers</t>
   </si>
   <si>
-    <t>Pole Number</t>
-  </si>
-  <si>
     <t>1 Byte number that identifies a pole uniquely</t>
   </si>
   <si>
-    <t>0x00 (Factory Default)</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -181,6 +175,21 @@
   </si>
   <si>
     <t>0x00000000_00000000 (Factory Default)</t>
+  </si>
+  <si>
+    <t>&lt;! Regular Registers&gt;</t>
+  </si>
+  <si>
+    <t>Pole ID</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>4 Byte unix time(Integer)</t>
+  </si>
+  <si>
+    <t>0xFF (Factory Default)</t>
   </si>
 </sst>
 </file>
@@ -533,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,12 +840,12 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B23">
         <v>11</v>
@@ -848,15 +857,15 @@
         <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>12</v>
@@ -868,10 +877,32 @@
         <v>15</v>
       </c>
       <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>53</v>
-      </c>
-      <c r="F24" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ADDED] Registers for RMS and energy
</commit_message>
<xml_diff>
--- a/Docu/registers.xlsx
+++ b/Docu/registers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Reg ID</t>
   </si>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>0xFF (Factory Default)</t>
+  </si>
+  <si>
+    <t>V and I</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>2*3*2 Bytes (Whr,VARhr,Vahr) (2 bytes each, two phase each AC and BC)</t>
+  </si>
+  <si>
+    <t>3*2*2 Bytes (VRMS, IRMS ) (3 bytes each, two phase each AC and BC)</t>
   </si>
 </sst>
 </file>
@@ -542,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +565,7 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="55.28515625" customWidth="1"/>
+    <col min="5" max="5" width="64.85546875" customWidth="1"/>
     <col min="6" max="6" width="53.140625" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
@@ -900,8 +912,42 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ADDED] Update functions for VRMS and IRMS register and Energy register.
</commit_message>
<xml_diff>
--- a/Docu/registers.xlsx
+++ b/Docu/registers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>Reg ID</t>
   </si>
@@ -198,10 +198,16 @@
     <t>Energy</t>
   </si>
   <si>
-    <t>2*3*2 Bytes (Whr,VARhr,Vahr) (2 bytes each, two phase each AC and BC)</t>
-  </si>
-  <si>
-    <t>3*2*2 Bytes (VRMS, IRMS ) (3 bytes each, two phase each AC and BC)</t>
+    <t>3*2*2 Bytes (VRMS, IRMS ) (3 bytes each, two phase each -&gt; AC and BC)</t>
+  </si>
+  <si>
+    <t>2*3*2 Bytes (Whr,VARhr,Vahr) (2 bytes each, two phase each -&gt; AC and BC)</t>
+  </si>
+  <si>
+    <t>1 byte Alert[bit7-0]=(overVoltage AC, overVoltage BC, under Voltage AC, under Voltage BC, overCurrent A, overCurrent B, 0, 0)</t>
+  </si>
+  <si>
+    <t>threshold of 3 bytes each corresponding to the above alerts.</t>
   </si>
 </sst>
 </file>
@@ -556,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,13 +926,13 @@
         <v>14</v>
       </c>
       <c r="C26">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -937,18 +943,38 @@
         <v>15</v>
       </c>
       <c r="C27">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
         <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
+      </c>
+      <c r="C29">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>